<commit_message>
fix(TB Export Xls) allow extended twig templates in xls
Change-Id: Ib4710c3d872b3bcec47bbcbdb6ec5e2e22f33280
Reviewed-on: http://gerrit.tine20.com/customers/19119
Tested-by: Jenkins CI (http://ci.tine20.com/) <tine20-jenkins@metaways.de>
Reviewed-by: Paul Mehrer <p.mehrer@metaways.de>
</commit_message>
<xml_diff>
--- a/tests/tine20/Tinebase/files/export/addressbook_contact_twigFunctions.xlsx
+++ b/tests/tine20/Tinebase/files/export/addressbook_contact_twigFunctions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">${twig:addNewLine(translate('Contact'))} ${twig:addNewLine(_('Contact'))} ${twig:ngettext('Contact', 'Contacts', 2)}</t>
   </si>
   <si>
     <t xml:space="preserve">${ROW}${twig:dateFormat(record.bday, 'date')}${/ROW}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${twig: {% if record.bday %} {{record.bday|date("m/d/Y")}}{% endif %} }</t>
   </si>
 </sst>
 </file>
@@ -180,15 +183,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="9.9962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -218,10 +221,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
fix(TB Export Xls) fix extended twig syntax (ifs)
Change-Id: I5b15e9cbb6c1728993283e0876de1903cb6465ba
Reviewed-on: http://gerrit.tine20.com/customers/19155
Tested-by: Jenkins CI (http://ci.tine20.com/) <tine20-jenkins@metaways.de>
Reviewed-by: Paul Mehrer <p.mehrer@metaways.de>
</commit_message>
<xml_diff>
--- a/tests/tine20/Tinebase/files/export/addressbook_contact_twigFunctions.xlsx
+++ b/tests/tine20/Tinebase/files/export/addressbook_contact_twigFunctions.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">${ROW}${twig:dateFormat(record.bday, 'date')}${/ROW}</t>
   </si>
   <si>
-    <t xml:space="preserve">${twig: {% if record.bday %} {{record.bday|date("m/d/Y")}}{% endif %} }</t>
+    <t xml:space="preserve">${twig: {% if record.bday %} {{record.bday|date("m/d/Y")=}{% endif %}}</t>
   </si>
 </sst>
 </file>
@@ -186,7 +186,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>